<commit_message>
calculation of t based on time base parameter deciphered P2
</commit_message>
<xml_diff>
--- a/notes/cmd4.xlsx
+++ b/notes/cmd4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-50280" yWindow="3740" windowWidth="38860" windowHeight="21640" tabRatio="500"/>
+    <workbookView xWindow="-55420" yWindow="9040" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt2" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="71">
   <si>
     <t>P1</t>
   </si>
@@ -145,18 +145,12 @@
     <t>(11,24mm)</t>
   </si>
   <si>
-    <t>P2 ???????????</t>
-  </si>
-  <si>
     <t>double P2 ==&gt; half speed</t>
   </si>
   <si>
     <t>half P2 ==&gt; double speed</t>
   </si>
   <si>
-    <t>t (msec)</t>
-  </si>
-  <si>
     <t>TESTMOVE:</t>
   </si>
   <si>
@@ -209,6 +203,36 @@
   </si>
   <si>
     <t>GRBL: planner + stepper ==&gt; calculation</t>
+  </si>
+  <si>
+    <t>PARA:$4B</t>
+  </si>
+  <si>
+    <t>t (units)</t>
+  </si>
+  <si>
+    <t>timebase</t>
+  </si>
+  <si>
+    <t>P1 = (time / 0,0005)+1.0</t>
+  </si>
+  <si>
+    <t>P2 = round_to_50s( 50000000 * time / P1 )</t>
+  </si>
+  <si>
+    <t>P2*854.0/50000000 = x...</t>
+  </si>
+  <si>
+    <t>P2*854.0/50000000 = y...</t>
+  </si>
+  <si>
+    <t>P2*40.0/50000000 = a...</t>
+  </si>
+  <si>
+    <t>CPU MHz?</t>
+  </si>
+  <si>
+    <t>a*t/50000000</t>
   </si>
 </sst>
 </file>
@@ -270,7 +294,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -302,8 +326,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -315,8 +349,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="41">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -332,6 +367,11 @@
     <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -347,6 +387,11 @@
     <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -676,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:W32"/>
+  <dimension ref="B1:W39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -687,7 +732,7 @@
     <col min="1" max="1" width="2.33203125" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.33203125" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
     <col min="8" max="8" width="7.83203125" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" customWidth="1"/>
     <col min="10" max="10" width="7.6640625" customWidth="1"/>
@@ -756,9 +801,11 @@
     </row>
     <row r="2" spans="2:23" s="3" customFormat="1">
       <c r="C2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="4"/>
+        <v>62</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="E2" s="4" t="s">
         <v>24</v>
       </c>
@@ -1473,9 +1520,26 @@
         <v>11.239500237851288</v>
       </c>
     </row>
+    <row r="15" spans="2:23">
+      <c r="E15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15">
+        <v>20000000</v>
+      </c>
+      <c r="G15" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="16" spans="2:23">
-      <c r="D16" t="s">
-        <v>41</v>
+      <c r="F16">
+        <v>50000000</v>
+      </c>
+      <c r="G16" t="s">
+        <v>61</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="Q16" t="s">
         <v>38</v>
@@ -1488,88 +1552,109 @@
       </c>
     </row>
     <row r="18" spans="2:16">
-      <c r="D18" t="s">
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16">
+      <c r="B19" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="19" spans="2:16">
-      <c r="D19" t="s">
+      <c r="F19" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16">
+      <c r="F21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16">
+      <c r="F22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16">
+      <c r="F23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16">
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16">
+      <c r="B32" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="22" spans="2:16">
-      <c r="B22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="2:16">
-      <c r="B25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E25" t="s">
-        <v>46</v>
-      </c>
-      <c r="G25" t="s">
-        <v>52</v>
-      </c>
-      <c r="I25" t="s">
-        <v>49</v>
-      </c>
-      <c r="M25" t="s">
-        <v>57</v>
-      </c>
-      <c r="N25">
+      <c r="E32" t="s">
+        <v>44</v>
+      </c>
+      <c r="G32" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" t="s">
+        <v>47</v>
+      </c>
+      <c r="M32" t="s">
+        <v>55</v>
+      </c>
+      <c r="N32">
         <f>100/1000</f>
         <v>0.1</v>
       </c>
-      <c r="O25" s="5" t="s">
+      <c r="O32" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="P32" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="P25" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="2:16">
-      <c r="E26" t="s">
-        <v>47</v>
-      </c>
-      <c r="G26" t="s">
+    </row>
+    <row r="33" spans="5:15">
+      <c r="E33" t="s">
+        <v>45</v>
+      </c>
+      <c r="G33" t="s">
+        <v>51</v>
+      </c>
+      <c r="I33" t="s">
+        <v>48</v>
+      </c>
+      <c r="M33" t="s">
         <v>53</v>
       </c>
-      <c r="I26" t="s">
-        <v>50</v>
-      </c>
-      <c r="M26" t="s">
-        <v>55</v>
-      </c>
-      <c r="N26">
+      <c r="N33">
         <f>50/1000</f>
         <v>0.05</v>
       </c>
-      <c r="O26" s="5" t="s">
+      <c r="O33" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="5:15">
+      <c r="E34" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" t="s">
+        <v>52</v>
+      </c>
+      <c r="I34" t="s">
+        <v>49</v>
+      </c>
+      <c r="M34" t="s">
+        <v>54</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="5:15">
+      <c r="G39" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="2:16">
-      <c r="E27" t="s">
-        <v>48</v>
-      </c>
-      <c r="G27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I27" t="s">
-        <v>51</v>
-      </c>
-      <c r="M27" t="s">
-        <v>56</v>
-      </c>
-      <c r="N27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:16">
-      <c r="G32" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added one more test sheet
</commit_message>
<xml_diff>
--- a/notes/cmd4.xlsx
+++ b/notes/cmd4.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-55420" yWindow="9040" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="-47320" yWindow="9460" windowWidth="28860" windowHeight="17880" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Blatt2" sheetId="2" r:id="rId1"/>
-    <sheet name="Blatt1" sheetId="1" r:id="rId2"/>
+    <sheet name="Blatt2 (2)" sheetId="3" r:id="rId1"/>
+    <sheet name="Blatt2" sheetId="2" r:id="rId2"/>
+    <sheet name="Blatt1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="72">
   <si>
     <t>P1</t>
   </si>
@@ -217,9 +218,6 @@
     <t>P1 = (time / 0,0005)+1.0</t>
   </si>
   <si>
-    <t>P2 = round_to_50s( 50000000 * time / P1 )</t>
-  </si>
-  <si>
     <t>P2*854.0/50000000 = x...</t>
   </si>
   <si>
@@ -233,6 +231,12 @@
   </si>
   <si>
     <t>a*t/50000000</t>
+  </si>
+  <si>
+    <t>P2 = round_to_50s( 20000000 * time / P1 )</t>
+  </si>
+  <si>
+    <t>(11,23mm)</t>
   </si>
 </sst>
 </file>
@@ -294,8 +298,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -351,7 +367,7 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="53">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -372,6 +388,12 @@
     <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -392,6 +414,12 @@
     <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -721,10 +749,2507 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:AA59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z32" sqref="Z32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="7.83203125" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" customWidth="1"/>
+    <col min="11" max="12" width="2.1640625" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="2" customWidth="1"/>
+    <col min="22" max="23" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="3.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:27" s="3" customFormat="1">
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="2:27" s="3" customFormat="1">
+      <c r="C2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="2:27">
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>24300</v>
+      </c>
+      <c r="E3">
+        <v>127</v>
+      </c>
+      <c r="F3">
+        <v>176</v>
+      </c>
+      <c r="G3">
+        <v>125</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>309</v>
+      </c>
+      <c r="J3">
+        <v>87</v>
+      </c>
+      <c r="M3" s="1">
+        <f t="shared" ref="M3:O31" si="0">H3/512</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <f t="shared" si="0"/>
+        <v>0.603515625</v>
+      </c>
+      <c r="O3" s="1">
+        <f t="shared" si="0"/>
+        <v>0.169921875</v>
+      </c>
+      <c r="Q3" s="7">
+        <f>($C3*E3+($C3*($C3-1))*H3/2-511)/512/854</f>
+        <v>-6.8610948477751756E-6</v>
+      </c>
+      <c r="R3" s="7">
+        <f>($C3*F3+($C3*($C3-1))*I3/2-511)/512/854</f>
+        <v>4.6815537177985946E-3</v>
+      </c>
+      <c r="S3" s="7">
+        <f>($C3*G3+($C3*($C3-1))*J3/2-511)/512/854</f>
+        <v>1.1686731557377049E-3</v>
+      </c>
+      <c r="U3" s="7">
+        <f>(E3+$C3*H3)/512</f>
+        <v>0.248046875</v>
+      </c>
+      <c r="V3" s="7">
+        <f t="shared" ref="V3:W31" si="1">(F3+$C3*I3)/512</f>
+        <v>2.7578125</v>
+      </c>
+      <c r="W3" s="7">
+        <f t="shared" si="1"/>
+        <v>0.923828125</v>
+      </c>
+      <c r="Z3">
+        <f>(C3-0.115)*0.0005</f>
+        <v>1.9425E-3</v>
+      </c>
+      <c r="AA3">
+        <f>ROUNDDOWN((50000000*Z3/C3+25)/50,0)*50</f>
+        <v>24300</v>
+      </c>
+    </row>
+    <row r="4" spans="2:27">
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>490</v>
+      </c>
+      <c r="D4">
+        <v>25000</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1275</v>
+      </c>
+      <c r="G4">
+        <v>359</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <f t="shared" ref="M4:M30" si="2">H4/512</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" ref="N4:N30" si="3">I4/512</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" ref="O4:O30" si="4">J4/512</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="7">
+        <f t="shared" ref="Q4:Q30" si="5">($C4*E4+($C4*($C4-1))*H4/2-511)/512/854</f>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R4" s="7">
+        <f t="shared" ref="R4:R30" si="6">($C4*F4+($C4*($C4-1))*I4/2-511)/512/854</f>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S4" s="7">
+        <f t="shared" ref="S4:S30" si="7">($C4*G4+($C4*($C4-1))*J4/2-511)/512/854</f>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U4" s="7">
+        <f t="shared" ref="U4:U30" si="8">(E4+$C4*H4)/512</f>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V4" s="7">
+        <f t="shared" ref="V4:V30" si="9">(F4+$C4*I4)/512</f>
+        <v>2.490234375</v>
+      </c>
+      <c r="W4" s="7">
+        <f t="shared" ref="W4:W30" si="10">(G4+$C4*J4)/512</f>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z4">
+        <f>(C4-0.115)*0.0005</f>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA4">
+        <f t="shared" ref="AA4:AA32" si="11">ROUNDDOWN((50000000*Z4/C4+25)/50,0)*50</f>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:27">
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>490</v>
+      </c>
+      <c r="D5">
+        <v>25000</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1275</v>
+      </c>
+      <c r="G5">
+        <v>358</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R5" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S5" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40002241290983609</v>
+      </c>
+      <c r="U5" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V5" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W5" s="7">
+        <f t="shared" si="10"/>
+        <v>0.69921875</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" ref="Z5:Z32" si="12">(C5-0.115)*0.0005</f>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA5">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:27">
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>490</v>
+      </c>
+      <c r="D6">
+        <v>25000</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1275</v>
+      </c>
+      <c r="G6">
+        <v>359</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R6" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S6" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U6" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V6" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W6" s="7">
+        <f t="shared" si="10"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA6">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:27">
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>490</v>
+      </c>
+      <c r="D7">
+        <v>25000</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1275</v>
+      </c>
+      <c r="G7">
+        <v>359</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R7" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S7" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U7" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V7" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W7" s="7">
+        <f t="shared" si="10"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA7">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:27">
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>490</v>
+      </c>
+      <c r="D8">
+        <v>25000</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1275</v>
+      </c>
+      <c r="G8">
+        <v>359</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R8" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S8" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U8" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V8" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W8" s="7">
+        <f t="shared" si="10"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA8">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:27">
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>490</v>
+      </c>
+      <c r="D9">
+        <v>25000</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1275</v>
+      </c>
+      <c r="G9">
+        <v>358</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R9" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S9" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40002241290983609</v>
+      </c>
+      <c r="U9" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V9" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W9" s="7">
+        <f t="shared" si="10"/>
+        <v>0.69921875</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA9">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:27">
+      <c r="B10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>490</v>
+      </c>
+      <c r="D10">
+        <v>25000</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1275</v>
+      </c>
+      <c r="G10">
+        <v>359</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R10" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S10" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U10" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V10" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W10" s="7">
+        <f t="shared" si="10"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA10">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:27">
+      <c r="B11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>490</v>
+      </c>
+      <c r="D11">
+        <v>25000</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1275</v>
+      </c>
+      <c r="G11">
+        <v>359</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R11" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S11" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U11" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V11" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W11" s="7">
+        <f t="shared" si="10"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA11">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:27">
+      <c r="B12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>490</v>
+      </c>
+      <c r="D12">
+        <v>25000</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1275</v>
+      </c>
+      <c r="G12">
+        <v>359</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R12" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S12" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U12" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V12" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W12" s="7">
+        <f t="shared" si="10"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:27">
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>490</v>
+      </c>
+      <c r="D13">
+        <v>25000</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1275</v>
+      </c>
+      <c r="G13">
+        <v>358</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R13" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S13" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40002241290983609</v>
+      </c>
+      <c r="U13" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V13" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W13" s="7">
+        <f t="shared" si="10"/>
+        <v>0.69921875</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA13">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="14" spans="2:27">
+      <c r="B14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>490</v>
+      </c>
+      <c r="D14">
+        <v>25000</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1275</v>
+      </c>
+      <c r="G14">
+        <v>359</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R14" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S14" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U14" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V14" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W14" s="7">
+        <f t="shared" si="10"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="15" spans="2:27">
+      <c r="B15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>490</v>
+      </c>
+      <c r="D15">
+        <v>25000</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1275</v>
+      </c>
+      <c r="G15">
+        <v>359</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R15" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S15" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U15" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V15" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W15" s="7">
+        <f t="shared" si="10"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA15">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="16" spans="2:27">
+      <c r="B16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>490</v>
+      </c>
+      <c r="D16">
+        <v>25000</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1275</v>
+      </c>
+      <c r="G16">
+        <v>359</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R16" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S16" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U16" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V16" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W16" s="7">
+        <f t="shared" si="10"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA16">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="17" spans="2:27">
+      <c r="B17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>490</v>
+      </c>
+      <c r="D17">
+        <v>25000</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1275</v>
+      </c>
+      <c r="G17">
+        <v>359</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="M17" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R17" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S17" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U17" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V17" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W17" s="7">
+        <f t="shared" si="10"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA17">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:27">
+      <c r="B18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>490</v>
+      </c>
+      <c r="D18">
+        <v>25000</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1275</v>
+      </c>
+      <c r="G18">
+        <v>358</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R18" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S18" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40002241290983609</v>
+      </c>
+      <c r="U18" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V18" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W18" s="7">
+        <f t="shared" si="10"/>
+        <v>0.69921875</v>
+      </c>
+      <c r="Z18">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA18">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="19" spans="2:27">
+      <c r="B19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>490</v>
+      </c>
+      <c r="D19">
+        <v>25000</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1275</v>
+      </c>
+      <c r="G19">
+        <v>359</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="M19" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R19" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S19" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U19" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V19" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W19" s="7">
+        <f t="shared" si="10"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z19">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA19">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:27">
+      <c r="B20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20">
+        <v>490</v>
+      </c>
+      <c r="D20">
+        <v>25000</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1275</v>
+      </c>
+      <c r="G20">
+        <v>359</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R20" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S20" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U20" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V20" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W20" s="7">
+        <f t="shared" si="10"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z20">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA20">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="21" spans="2:27">
+      <c r="B21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21">
+        <v>490</v>
+      </c>
+      <c r="D21">
+        <v>25000</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1275</v>
+      </c>
+      <c r="G21">
+        <v>359</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O21" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R21" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S21" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U21" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V21" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W21" s="7">
+        <f t="shared" si="10"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z21">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA21">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="22" spans="2:27">
+      <c r="B22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>490</v>
+      </c>
+      <c r="D22">
+        <v>25000</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1275</v>
+      </c>
+      <c r="G22">
+        <v>358</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O22" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R22" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S22" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40002241290983609</v>
+      </c>
+      <c r="U22" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V22" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W22" s="7">
+        <f t="shared" si="10"/>
+        <v>0.69921875</v>
+      </c>
+      <c r="Z22">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA22">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="23" spans="2:27">
+      <c r="B23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23">
+        <v>490</v>
+      </c>
+      <c r="D23">
+        <v>25000</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1275</v>
+      </c>
+      <c r="G23">
+        <v>359</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="M23" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N23" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O23" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R23" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S23" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U23" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V23" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W23" s="7">
+        <f t="shared" si="10"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z23">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA23">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="24" spans="2:27">
+      <c r="B24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24">
+        <v>490</v>
+      </c>
+      <c r="D24">
+        <v>25000</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1275</v>
+      </c>
+      <c r="G24">
+        <v>359</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="M24" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N24" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O24" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R24" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S24" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U24" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V24" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W24" s="7">
+        <f t="shared" si="10"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z24">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA24">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="25" spans="2:27">
+      <c r="B25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25">
+        <v>490</v>
+      </c>
+      <c r="D25">
+        <v>25000</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1275</v>
+      </c>
+      <c r="G25">
+        <v>359</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="M25" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N25" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O25" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R25" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S25" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U25" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V25" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W25" s="7">
+        <f t="shared" si="10"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z25">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA25">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="26" spans="2:27">
+      <c r="B26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26">
+        <v>490</v>
+      </c>
+      <c r="D26">
+        <v>25000</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1275</v>
+      </c>
+      <c r="G26">
+        <v>358</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="M26" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N26" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O26" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q26" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R26" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S26" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40002241290983609</v>
+      </c>
+      <c r="U26" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V26" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W26" s="7">
+        <f t="shared" si="10"/>
+        <v>0.69921875</v>
+      </c>
+      <c r="Z26">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA26">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="27" spans="2:27">
+      <c r="B27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27">
+        <v>490</v>
+      </c>
+      <c r="D27">
+        <v>25000</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1275</v>
+      </c>
+      <c r="G27">
+        <v>359</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="M27" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N27" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O27" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R27" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S27" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U27" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V27" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W27" s="7">
+        <f t="shared" si="10"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z27">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA27">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="28" spans="2:27">
+      <c r="B28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28">
+        <v>490</v>
+      </c>
+      <c r="D28">
+        <v>25000</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1275</v>
+      </c>
+      <c r="G28">
+        <v>359</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="M28" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N28" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O28" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R28" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S28" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U28" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V28" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W28" s="7">
+        <f t="shared" si="10"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z28">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA28">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="29" spans="2:27">
+      <c r="B29" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29">
+        <v>490</v>
+      </c>
+      <c r="D29">
+        <v>25000</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1275</v>
+      </c>
+      <c r="G29">
+        <v>359</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="M29" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O29" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R29" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S29" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U29" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V29" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W29" s="7">
+        <f t="shared" si="10"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z29">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA29">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="30" spans="2:27">
+      <c r="B30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30">
+        <v>490</v>
+      </c>
+      <c r="D30">
+        <v>25000</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1275</v>
+      </c>
+      <c r="G30">
+        <v>358</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="M30" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N30" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O30" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q30" s="7">
+        <f t="shared" si="5"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R30" s="7">
+        <f t="shared" si="6"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S30" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40002241290983609</v>
+      </c>
+      <c r="U30" s="7">
+        <f t="shared" si="8"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V30" s="7">
+        <f t="shared" si="9"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W30" s="7">
+        <f t="shared" si="10"/>
+        <v>0.69921875</v>
+      </c>
+      <c r="Z30">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA30">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="31" spans="2:27">
+      <c r="B31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31">
+        <v>490</v>
+      </c>
+      <c r="D31">
+        <v>25000</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>1275</v>
+      </c>
+      <c r="G31">
+        <v>359</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="M31" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N31" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O31" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q31" s="7">
+        <f t="shared" ref="Q31:S31" si="13">($C31*E31+($C31*($C31-1))*H31/2-511)/512/854</f>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R31" s="7">
+        <f t="shared" si="13"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S31" s="7">
+        <f t="shared" si="13"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U31" s="7">
+        <f t="shared" ref="U31" si="14">(E31+$C31*H31)/512</f>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V31" s="7">
+        <f t="shared" si="1"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W31" s="7">
+        <f t="shared" si="1"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z31">
+        <f t="shared" si="12"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA31">
+        <f t="shared" si="11"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="32" spans="2:27">
+      <c r="B32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <v>24300</v>
+      </c>
+      <c r="E32">
+        <v>127</v>
+      </c>
+      <c r="F32">
+        <v>1231</v>
+      </c>
+      <c r="G32">
+        <v>386</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>-309</v>
+      </c>
+      <c r="J32">
+        <v>-87</v>
+      </c>
+      <c r="M32" s="1">
+        <f t="shared" ref="M32" si="15">H32/512</f>
+        <v>0</v>
+      </c>
+      <c r="N32" s="1">
+        <f t="shared" ref="N32" si="16">I32/512</f>
+        <v>-0.603515625</v>
+      </c>
+      <c r="O32" s="1">
+        <f t="shared" ref="O32" si="17">J32/512</f>
+        <v>-0.169921875</v>
+      </c>
+      <c r="Q32" s="7">
+        <f t="shared" ref="Q32" si="18">($C32*E32+($C32*($C32-1))*H32/2-511)/512/854</f>
+        <v>-6.8610948477751756E-6</v>
+      </c>
+      <c r="R32" s="7">
+        <f t="shared" ref="R32" si="19">($C32*F32+($C32*($C32-1))*I32/2-511)/512/854</f>
+        <v>5.852513905152225E-3</v>
+      </c>
+      <c r="S32" s="7">
+        <f t="shared" ref="S32" si="20">($C32*G32+($C32*($C32-1))*J32/2-511)/512/854</f>
+        <v>1.1686731557377049E-3</v>
+      </c>
+      <c r="U32" s="7">
+        <f t="shared" ref="U32" si="21">(E32+$C32*H32)/512</f>
+        <v>0.248046875</v>
+      </c>
+      <c r="V32" s="7">
+        <f t="shared" ref="V32" si="22">(F32+$C32*I32)/512</f>
+        <v>-9.765625E-3</v>
+      </c>
+      <c r="W32" s="7">
+        <f t="shared" ref="W32" si="23">(G32+$C32*J32)/512</f>
+        <v>7.421875E-2</v>
+      </c>
+      <c r="Z32">
+        <f t="shared" si="12"/>
+        <v>1.9425E-3</v>
+      </c>
+      <c r="AA32">
+        <f t="shared" si="11"/>
+        <v>24300</v>
+      </c>
+    </row>
+    <row r="34" spans="2:26">
+      <c r="C34">
+        <f>SUM(C3:C33)</f>
+        <v>13728</v>
+      </c>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="N34" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P34" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q34" s="8">
+        <f>SUM(Q3:Q31)</f>
+        <v>-1.3516356850117105E-3</v>
+      </c>
+      <c r="R34" s="8">
+        <f>SUM(R3:R31)</f>
+        <v>39.979002762734183</v>
+      </c>
+      <c r="S34" s="8">
+        <f>SUM(S3:S31)</f>
+        <v>11.225329789959016</v>
+      </c>
+      <c r="Z34" s="3">
+        <f>SUM(Z3:Z33)</f>
+        <v>6.8622749999999968</v>
+      </c>
+    </row>
+    <row r="35" spans="2:26">
+      <c r="E35" t="s">
+        <v>68</v>
+      </c>
+      <c r="F35">
+        <v>20000000</v>
+      </c>
+      <c r="G35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="2:26">
+      <c r="F36">
+        <v>50000000</v>
+      </c>
+      <c r="G36" t="s">
+        <v>61</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>38</v>
+      </c>
+      <c r="R36" t="s">
+        <v>39</v>
+      </c>
+      <c r="S36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="2:26">
+      <c r="B38" t="s">
+        <v>41</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="2:26">
+      <c r="B39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="2:26">
+      <c r="F41" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="2:26">
+      <c r="F42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="2:26">
+      <c r="F43" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="2:16">
+      <c r="B49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="2:16">
+      <c r="N50" s="3"/>
+    </row>
+    <row r="52" spans="2:16">
+      <c r="B52" t="s">
+        <v>43</v>
+      </c>
+      <c r="E52" t="s">
+        <v>44</v>
+      </c>
+      <c r="G52" t="s">
+        <v>50</v>
+      </c>
+      <c r="I52" t="s">
+        <v>47</v>
+      </c>
+      <c r="M52" t="s">
+        <v>55</v>
+      </c>
+      <c r="N52">
+        <f>100/1000</f>
+        <v>0.1</v>
+      </c>
+      <c r="O52" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="P52" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="2:16">
+      <c r="E53" t="s">
+        <v>45</v>
+      </c>
+      <c r="G53" t="s">
+        <v>51</v>
+      </c>
+      <c r="I53" t="s">
+        <v>48</v>
+      </c>
+      <c r="M53" t="s">
+        <v>53</v>
+      </c>
+      <c r="N53">
+        <f>50/1000</f>
+        <v>0.05</v>
+      </c>
+      <c r="O53" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="2:16">
+      <c r="E54" t="s">
+        <v>46</v>
+      </c>
+      <c r="G54" t="s">
+        <v>52</v>
+      </c>
+      <c r="I54" t="s">
+        <v>49</v>
+      </c>
+      <c r="M54" t="s">
+        <v>54</v>
+      </c>
+      <c r="N54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:16">
+      <c r="G59" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1522,7 +4047,7 @@
     </row>
     <row r="15" spans="2:23">
       <c r="E15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F15">
         <v>20000000</v>
@@ -1539,7 +4064,7 @@
         <v>61</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q16" t="s">
         <v>38</v>
@@ -1564,27 +4089,125 @@
         <v>42</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>65</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16">
+      <c r="N20">
+        <f>(C3-1)*0.0005</f>
+        <v>6.5000000000000006E-3</v>
+      </c>
+      <c r="O20">
+        <f>ROUNDDOWN((20000000*N20/C3+25)/50,0)*50</f>
+        <v>9300</v>
       </c>
     </row>
     <row r="21" spans="2:16">
       <c r="F21" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="N21">
+        <f t="shared" ref="N21:N29" si="9">(C4-1)*0.0005</f>
+        <v>0.249</v>
+      </c>
+      <c r="O21">
+        <f t="shared" ref="O21:O30" si="10">ROUNDDOWN((20000000*N21/C4+25)/50,0)*50</f>
+        <v>10000</v>
       </c>
     </row>
     <row r="22" spans="2:16">
       <c r="F22" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="9"/>
+        <v>0.249</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="10"/>
+        <v>10000</v>
       </c>
     </row>
     <row r="23" spans="2:16">
       <c r="F23" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="9"/>
+        <v>0.249</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="10"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16">
+      <c r="N24">
+        <f t="shared" si="9"/>
+        <v>0.249</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="10"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16">
+      <c r="N25">
+        <f t="shared" si="9"/>
+        <v>0.249</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="10"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16">
+      <c r="N26">
+        <f t="shared" si="9"/>
+        <v>0.249</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="10"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16">
+      <c r="N27">
+        <f t="shared" si="9"/>
+        <v>0.249</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="10"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16">
+      <c r="N28">
+        <f t="shared" si="9"/>
+        <v>0.249</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="10"/>
+        <v>10000</v>
       </c>
     </row>
     <row r="29" spans="2:16">
       <c r="B29" t="s">
         <v>60</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="9"/>
+        <v>6.5000000000000006E-3</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="10"/>
+        <v>9300</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16">
+      <c r="N30" s="3">
+        <f>SUM(N20:N29)</f>
+        <v>2.0050000000000003</v>
       </c>
     </row>
     <row r="32" spans="2:16">
@@ -1668,7 +4291,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L47"/>
   <sheetViews>

</xml_diff>

<commit_message>
added some commands and descriptions
</commit_message>
<xml_diff>
--- a/notes/cmd4.xlsx
+++ b/notes/cmd4.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-47320" yWindow="9460" windowWidth="28860" windowHeight="17880" tabRatio="500"/>
+    <workbookView xWindow="-46880" yWindow="6380" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt2 (2)" sheetId="3" r:id="rId1"/>
     <sheet name="Blatt2" sheetId="2" r:id="rId2"/>
     <sheet name="Blatt1" sheetId="1" r:id="rId3"/>
+    <sheet name="Blatt3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="79">
   <si>
     <t>P1</t>
   </si>
@@ -237,6 +238,27 @@
   </si>
   <si>
     <t>(11,23mm)</t>
+  </si>
+  <si>
+    <t>P2 = round_to_50s( 50000000 * time / P1 )</t>
+  </si>
+  <si>
+    <t>program 5</t>
+  </si>
+  <si>
+    <t>every 6.25 micro seconds one pulse</t>
+  </si>
+  <si>
+    <t>160khz</t>
+  </si>
+  <si>
+    <t>program5</t>
+  </si>
+  <si>
+    <t>every 2.528</t>
+  </si>
+  <si>
+    <t>400khZ</t>
   </si>
 </sst>
 </file>
@@ -751,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AA59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z32" sqref="Z32"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3137,7 +3159,7 @@
         <v>42</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="2:26">
@@ -3248,7 +3270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W39"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
@@ -4111,7 +4133,7 @@
         <v>0.249</v>
       </c>
       <c r="O21">
-        <f t="shared" ref="O21:O30" si="10">ROUNDDOWN((20000000*N21/C4+25)/50,0)*50</f>
+        <f t="shared" ref="O21:O29" si="10">ROUNDDOWN((20000000*N21/C4+25)/50,0)*50</f>
         <v>10000</v>
       </c>
     </row>
@@ -5023,4 +5045,54 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:K4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="3" spans="2:11">
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="1">
+        <f>1/6.25</f>
+        <v>0.16</v>
+      </c>
+      <c r="K3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11">
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4">
+        <f>1/2.528</f>
+        <v>0.39556962025316456</v>
+      </c>
+      <c r="K4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
deciphered CMD 4 - YEAAAAHHHH !
</commit_message>
<xml_diff>
--- a/notes/cmd4.xlsx
+++ b/notes/cmd4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-46880" yWindow="6380" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-59260" yWindow="580" windowWidth="47160" windowHeight="19420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt2 (2)" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="88">
   <si>
     <t>P1</t>
   </si>
@@ -259,6 +259,33 @@
   </si>
   <si>
     <t>400khZ</t>
+  </si>
+  <si>
+    <t>50000000/25000 = 2000</t>
+  </si>
+  <si>
+    <t>1/0,0005 = 2000</t>
+  </si>
+  <si>
+    <t>timer freq?</t>
+  </si>
+  <si>
+    <t>t==&gt; timer events ?</t>
+  </si>
+  <si>
+    <t>(40,009 mm)</t>
+  </si>
+  <si>
+    <t>(4)</t>
+  </si>
+  <si>
+    <t>(5)</t>
+  </si>
+  <si>
+    <t>(34169)</t>
+  </si>
+  <si>
+    <t>steps/t</t>
   </si>
 </sst>
 </file>
@@ -320,7 +347,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -374,8 +401,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -388,8 +423,11 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="61">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -416,6 +454,10 @@
     <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -442,6 +484,10 @@
     <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -771,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AA59"/>
+  <dimension ref="B1:AM59"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Z3" sqref="Z3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AD3" sqref="AD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -796,7 +842,7 @@
     <col min="24" max="25" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:27" s="3" customFormat="1">
+    <row r="1" spans="2:39" s="3" customFormat="1">
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
@@ -850,7 +896,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="2:27" s="3" customFormat="1">
+    <row r="2" spans="2:39" s="3" customFormat="1">
       <c r="C2" s="4" t="s">
         <v>62</v>
       </c>
@@ -858,7 +904,7 @@
         <v>63</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>25</v>
@@ -894,7 +940,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="2:27">
+    <row r="3" spans="2:39">
       <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
@@ -908,7 +954,7 @@
         <v>127</v>
       </c>
       <c r="F3">
-        <v>176</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>125</v>
@@ -940,7 +986,7 @@
       </c>
       <c r="R3" s="7">
         <f>($C3*F3+($C3*($C3-1))*I3/2-511)/512/854</f>
-        <v>4.6815537177985946E-3</v>
+        <v>3.0714834601873538E-3</v>
       </c>
       <c r="S3" s="7">
         <f>($C3*G3+($C3*($C3-1))*J3/2-511)/512/854</f>
@@ -952,7 +998,7 @@
       </c>
       <c r="V3" s="7">
         <f t="shared" ref="V3:W31" si="1">(F3+$C3*I3)/512</f>
-        <v>2.7578125</v>
+        <v>2.4140625</v>
       </c>
       <c r="W3" s="7">
         <f t="shared" si="1"/>
@@ -966,8 +1012,42 @@
         <f>ROUNDDOWN((50000000*Z3/C3+25)/50,0)*50</f>
         <v>24300</v>
       </c>
-    </row>
-    <row r="4" spans="2:27">
+      <c r="AC3">
+        <f>C3</f>
+        <v>4</v>
+      </c>
+      <c r="AD3">
+        <f>($AC3*F3+(($AC3)*($AC3))*I3/2)/512</f>
+        <v>4.828125</v>
+      </c>
+      <c r="AE3">
+        <f t="shared" ref="AE3:AE32" si="2">ROUNDDOWN(AD3,0)</f>
+        <v>4</v>
+      </c>
+      <c r="AF3" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <f t="shared" ref="AJ3" si="3">F3/512</f>
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <f>AJ3*4</f>
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <f>(176+AH4+AH5+AH6)/512</f>
+        <v>3.96484375</v>
+      </c>
+      <c r="AM3">
+        <f>(309*4*4/2)/512</f>
+        <v>4.828125</v>
+      </c>
+    </row>
+    <row r="4" spans="2:39">
       <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
@@ -996,39 +1076,39 @@
         <v>0</v>
       </c>
       <c r="M4" s="1">
-        <f t="shared" ref="M4:M30" si="2">H4/512</f>
+        <f t="shared" ref="M4:M30" si="4">H4/512</f>
         <v>0</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" ref="N4:N30" si="3">I4/512</f>
+        <f t="shared" ref="N4:N30" si="5">I4/512</f>
         <v>0</v>
       </c>
       <c r="O4" s="1">
-        <f t="shared" ref="O4:O30" si="4">J4/512</f>
+        <f t="shared" ref="O4:O30" si="6">J4/512</f>
         <v>0</v>
       </c>
       <c r="Q4" s="7">
-        <f t="shared" ref="Q4:Q30" si="5">($C4*E4+($C4*($C4-1))*H4/2-511)/512/854</f>
+        <f t="shared" ref="Q4:Q30" si="7">($C4*E4+($C4*($C4-1))*H4/2-511)/512/854</f>
         <v>-4.8027663934426229E-5</v>
       </c>
       <c r="R4" s="7">
-        <f t="shared" ref="R4:R30" si="6">($C4*F4+($C4*($C4-1))*I4/2-511)/512/854</f>
+        <f t="shared" ref="R4:R30" si="8">($C4*F4+($C4*($C4-1))*I4/2-511)/512/854</f>
         <v>1.4276543288934427</v>
       </c>
       <c r="S4" s="7">
-        <f t="shared" ref="S4:S30" si="7">($C4*G4+($C4*($C4-1))*J4/2-511)/512/854</f>
+        <f t="shared" ref="S4:S30" si="9">($C4*G4+($C4*($C4-1))*J4/2-511)/512/854</f>
         <v>0.40114305840163933</v>
       </c>
       <c r="U4" s="7">
-        <f t="shared" ref="U4:U30" si="8">(E4+$C4*H4)/512</f>
+        <f t="shared" ref="U4:U30" si="10">(E4+$C4*H4)/512</f>
         <v>1.953125E-3</v>
       </c>
       <c r="V4" s="7">
-        <f t="shared" ref="V4:V30" si="9">(F4+$C4*I4)/512</f>
+        <f t="shared" ref="V4:V30" si="11">(F4+$C4*I4)/512</f>
         <v>2.490234375</v>
       </c>
       <c r="W4" s="7">
-        <f t="shared" ref="W4:W30" si="10">(G4+$C4*J4)/512</f>
+        <f t="shared" ref="W4:W30" si="12">(G4+$C4*J4)/512</f>
         <v>0.701171875</v>
       </c>
       <c r="Z4">
@@ -1036,11 +1116,34 @@
         <v>0.24494250000000001</v>
       </c>
       <c r="AA4">
-        <f t="shared" ref="AA4:AA32" si="11">ROUNDDOWN((50000000*Z4/C4+25)/50,0)*50</f>
+        <f t="shared" ref="AA4:AA32" si="13">ROUNDDOWN((50000000*Z4/C4+25)/50,0)*50</f>
         <v>25000</v>
       </c>
-    </row>
-    <row r="5" spans="2:27">
+      <c r="AC4">
+        <v>490</v>
+      </c>
+      <c r="AD4">
+        <f t="shared" ref="AD4:AD32" si="14">($AC4*F4+(($AC4)*($AC4))*I4/2)/512</f>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE4">
+        <f t="shared" si="2"/>
+        <v>1220</v>
+      </c>
+      <c r="AH4">
+        <f>AH3+309</f>
+        <v>309</v>
+      </c>
+      <c r="AJ4">
+        <f>F4/512</f>
+        <v>2.490234375</v>
+      </c>
+      <c r="AK4">
+        <f>AJ4*490</f>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="5" spans="2:39">
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1069,51 +1172,75 @@
         <v>0</v>
       </c>
       <c r="M5" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R5" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S5" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40002241290983609</v>
+      </c>
+      <c r="U5" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V5" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W5" s="7">
+        <f t="shared" si="12"/>
+        <v>0.69921875</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" ref="Z5:Z32" si="15">(C5-0.115)*0.0005</f>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA5">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC5">
+        <f t="shared" ref="AC4:AC32" si="16">C5</f>
+        <v>490</v>
+      </c>
+      <c r="AD5">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE5">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N5" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O5" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R5" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S5" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40002241290983609</v>
-      </c>
-      <c r="U5" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V5" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AH5">
+        <f t="shared" ref="AH5:AH7" si="17">AH4+309</f>
+        <v>618</v>
+      </c>
+      <c r="AJ5">
+        <f t="shared" ref="AJ5:AJ32" si="18">F5/512</f>
         <v>2.490234375</v>
       </c>
-      <c r="W5" s="7">
-        <f t="shared" si="10"/>
-        <v>0.69921875</v>
-      </c>
-      <c r="Z5">
-        <f t="shared" ref="Z5:Z32" si="12">(C5-0.115)*0.0005</f>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA5">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="6" spans="2:27">
+      <c r="AK5">
+        <f t="shared" ref="AK5:AK32" si="19">AJ5*490</f>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="6" spans="2:39">
       <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
@@ -1142,51 +1269,75 @@
         <v>0</v>
       </c>
       <c r="M6" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R6" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S6" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U6" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V6" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W6" s="7">
+        <f t="shared" si="12"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA6">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC6">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD6">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N6" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O6" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R6" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S6" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40114305840163933</v>
-      </c>
-      <c r="U6" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V6" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AH6">
+        <f t="shared" si="17"/>
+        <v>927</v>
+      </c>
+      <c r="AJ6">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W6" s="7">
-        <f t="shared" si="10"/>
-        <v>0.701171875</v>
-      </c>
-      <c r="Z6">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA6">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="7" spans="2:27">
+      <c r="AK6">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="7" spans="2:39">
       <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1215,51 +1366,75 @@
         <v>0</v>
       </c>
       <c r="M7" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R7" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S7" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U7" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V7" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W7" s="7">
+        <f t="shared" si="12"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA7">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC7">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD7">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N7" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O7" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R7" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S7" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40114305840163933</v>
-      </c>
-      <c r="U7" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V7" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AH7">
+        <f t="shared" si="17"/>
+        <v>1236</v>
+      </c>
+      <c r="AJ7">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W7" s="7">
-        <f t="shared" si="10"/>
-        <v>0.701171875</v>
-      </c>
-      <c r="Z7">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA7">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="8" spans="2:27">
+      <c r="AK7">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="8" spans="2:39">
       <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
@@ -1288,51 +1463,71 @@
         <v>0</v>
       </c>
       <c r="M8" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R8" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S8" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U8" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V8" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W8" s="7">
+        <f t="shared" si="12"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA8">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC8">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD8">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE8">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N8" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O8" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R8" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S8" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40114305840163933</v>
-      </c>
-      <c r="U8" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V8" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ8">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W8" s="7">
-        <f t="shared" si="10"/>
-        <v>0.701171875</v>
-      </c>
-      <c r="Z8">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA8">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="9" spans="2:27">
+      <c r="AK8">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="9" spans="2:39">
       <c r="B9" s="3" t="s">
         <v>12</v>
       </c>
@@ -1361,51 +1556,71 @@
         <v>0</v>
       </c>
       <c r="M9" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R9" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S9" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40002241290983609</v>
+      </c>
+      <c r="U9" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V9" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W9" s="7">
+        <f t="shared" si="12"/>
+        <v>0.69921875</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA9">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC9">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD9">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE9">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N9" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O9" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R9" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S9" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40002241290983609</v>
-      </c>
-      <c r="U9" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V9" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ9">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W9" s="7">
-        <f t="shared" si="10"/>
-        <v>0.69921875</v>
-      </c>
-      <c r="Z9">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA9">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="10" spans="2:27">
+      <c r="AK9">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="10" spans="2:39">
       <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
@@ -1434,51 +1649,71 @@
         <v>0</v>
       </c>
       <c r="M10" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R10" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S10" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U10" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V10" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W10" s="7">
+        <f t="shared" si="12"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA10">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC10">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE10">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N10" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O10" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q10" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R10" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S10" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40114305840163933</v>
-      </c>
-      <c r="U10" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V10" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ10">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W10" s="7">
-        <f t="shared" si="10"/>
-        <v>0.701171875</v>
-      </c>
-      <c r="Z10">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA10">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="11" spans="2:27">
+      <c r="AK10">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="11" spans="2:39">
       <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
@@ -1507,51 +1742,71 @@
         <v>0</v>
       </c>
       <c r="M11" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R11" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S11" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U11" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V11" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W11" s="7">
+        <f t="shared" si="12"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA11">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC11">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD11">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE11">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R11" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S11" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40114305840163933</v>
-      </c>
-      <c r="U11" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V11" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ11">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W11" s="7">
-        <f t="shared" si="10"/>
-        <v>0.701171875</v>
-      </c>
-      <c r="Z11">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA11">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="12" spans="2:27">
+      <c r="AK11">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="12" spans="2:39">
       <c r="B12" s="3" t="s">
         <v>12</v>
       </c>
@@ -1580,51 +1835,71 @@
         <v>0</v>
       </c>
       <c r="M12" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R12" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S12" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U12" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V12" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W12" s="7">
+        <f t="shared" si="12"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC12">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE12">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N12" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O12" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R12" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S12" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40114305840163933</v>
-      </c>
-      <c r="U12" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V12" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ12">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W12" s="7">
-        <f t="shared" si="10"/>
-        <v>0.701171875</v>
-      </c>
-      <c r="Z12">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA12">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="13" spans="2:27">
+      <c r="AK12">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="13" spans="2:39">
       <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
@@ -1653,51 +1928,71 @@
         <v>0</v>
       </c>
       <c r="M13" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R13" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S13" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40002241290983609</v>
+      </c>
+      <c r="U13" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V13" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W13" s="7">
+        <f t="shared" si="12"/>
+        <v>0.69921875</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA13">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC13">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD13">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE13">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N13" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R13" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S13" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40002241290983609</v>
-      </c>
-      <c r="U13" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V13" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ13">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W13" s="7">
-        <f t="shared" si="10"/>
-        <v>0.69921875</v>
-      </c>
-      <c r="Z13">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA13">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="14" spans="2:27">
+      <c r="AK13">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="14" spans="2:39">
       <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
@@ -1726,51 +2021,71 @@
         <v>0</v>
       </c>
       <c r="M14" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R14" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S14" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U14" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V14" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W14" s="7">
+        <f t="shared" si="12"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC14">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD14">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE14">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N14" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O14" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R14" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S14" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40114305840163933</v>
-      </c>
-      <c r="U14" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V14" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ14">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W14" s="7">
-        <f t="shared" si="10"/>
-        <v>0.701171875</v>
-      </c>
-      <c r="Z14">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA14">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="15" spans="2:27">
+      <c r="AK14">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="15" spans="2:39">
       <c r="B15" s="3" t="s">
         <v>12</v>
       </c>
@@ -1799,51 +2114,71 @@
         <v>0</v>
       </c>
       <c r="M15" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R15" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S15" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U15" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V15" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W15" s="7">
+        <f t="shared" si="12"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA15">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC15">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD15">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N15" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O15" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R15" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S15" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40114305840163933</v>
-      </c>
-      <c r="U15" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V15" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ15">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W15" s="7">
-        <f t="shared" si="10"/>
-        <v>0.701171875</v>
-      </c>
-      <c r="Z15">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA15">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="16" spans="2:27">
+      <c r="AK15">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="16" spans="2:39">
       <c r="B16" s="3" t="s">
         <v>12</v>
       </c>
@@ -1872,51 +2207,71 @@
         <v>0</v>
       </c>
       <c r="M16" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R16" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S16" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U16" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V16" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W16" s="7">
+        <f t="shared" si="12"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA16">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC16">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD16">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE16">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N16" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O16" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q16" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R16" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S16" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40114305840163933</v>
-      </c>
-      <c r="U16" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V16" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ16">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W16" s="7">
-        <f t="shared" si="10"/>
-        <v>0.701171875</v>
-      </c>
-      <c r="Z16">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA16">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="17" spans="2:27">
+      <c r="AK16">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="17" spans="2:39">
       <c r="B17" s="3" t="s">
         <v>12</v>
       </c>
@@ -1945,51 +2300,71 @@
         <v>0</v>
       </c>
       <c r="M17" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R17" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S17" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U17" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V17" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W17" s="7">
+        <f t="shared" si="12"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA17">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC17">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD17">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE17">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N17" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q17" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R17" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S17" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40114305840163933</v>
-      </c>
-      <c r="U17" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V17" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ17">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W17" s="7">
-        <f t="shared" si="10"/>
-        <v>0.701171875</v>
-      </c>
-      <c r="Z17">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA17">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="18" spans="2:27">
+      <c r="AK17">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="18" spans="2:39">
       <c r="B18" s="3" t="s">
         <v>12</v>
       </c>
@@ -2018,51 +2393,71 @@
         <v>0</v>
       </c>
       <c r="M18" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R18" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S18" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40002241290983609</v>
+      </c>
+      <c r="U18" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V18" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W18" s="7">
+        <f t="shared" si="12"/>
+        <v>0.69921875</v>
+      </c>
+      <c r="Z18">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA18">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC18">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD18">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE18">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N18" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O18" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q18" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R18" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S18" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40002241290983609</v>
-      </c>
-      <c r="U18" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V18" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ18">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W18" s="7">
-        <f t="shared" si="10"/>
-        <v>0.69921875</v>
-      </c>
-      <c r="Z18">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA18">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="19" spans="2:27">
+      <c r="AK18">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="19" spans="2:39">
       <c r="B19" s="3" t="s">
         <v>12</v>
       </c>
@@ -2091,51 +2486,71 @@
         <v>0</v>
       </c>
       <c r="M19" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R19" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S19" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U19" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V19" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W19" s="7">
+        <f t="shared" si="12"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z19">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA19">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC19">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD19">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE19">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N19" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O19" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R19" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S19" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40114305840163933</v>
-      </c>
-      <c r="U19" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V19" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ19">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W19" s="7">
-        <f t="shared" si="10"/>
-        <v>0.701171875</v>
-      </c>
-      <c r="Z19">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA19">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="20" spans="2:27">
+      <c r="AK19">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="20" spans="2:39">
       <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
@@ -2164,51 +2579,71 @@
         <v>0</v>
       </c>
       <c r="M20" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R20" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S20" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U20" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V20" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W20" s="7">
+        <f t="shared" si="12"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z20">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA20">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC20">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD20">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N20" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O20" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q20" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R20" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S20" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40114305840163933</v>
-      </c>
-      <c r="U20" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V20" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ20">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W20" s="7">
-        <f t="shared" si="10"/>
-        <v>0.701171875</v>
-      </c>
-      <c r="Z20">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA20">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="21" spans="2:27">
+      <c r="AK20">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="21" spans="2:39">
       <c r="B21" s="3" t="s">
         <v>12</v>
       </c>
@@ -2237,51 +2672,71 @@
         <v>0</v>
       </c>
       <c r="M21" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O21" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R21" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S21" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U21" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V21" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W21" s="7">
+        <f t="shared" si="12"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z21">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA21">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC21">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD21">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE21">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N21" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O21" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R21" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S21" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40114305840163933</v>
-      </c>
-      <c r="U21" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V21" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ21">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W21" s="7">
-        <f t="shared" si="10"/>
-        <v>0.701171875</v>
-      </c>
-      <c r="Z21">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA21">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="22" spans="2:27">
+      <c r="AK21">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="22" spans="2:39">
       <c r="B22" s="3" t="s">
         <v>12</v>
       </c>
@@ -2310,51 +2765,71 @@
         <v>0</v>
       </c>
       <c r="M22" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O22" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R22" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S22" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40002241290983609</v>
+      </c>
+      <c r="U22" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V22" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W22" s="7">
+        <f t="shared" si="12"/>
+        <v>0.69921875</v>
+      </c>
+      <c r="Z22">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA22">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC22">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD22">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE22">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N22" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O22" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q22" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R22" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S22" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40002241290983609</v>
-      </c>
-      <c r="U22" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V22" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ22">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W22" s="7">
-        <f t="shared" si="10"/>
-        <v>0.69921875</v>
-      </c>
-      <c r="Z22">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA22">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="23" spans="2:27">
+      <c r="AK22">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="23" spans="2:39">
       <c r="B23" s="3" t="s">
         <v>12</v>
       </c>
@@ -2383,51 +2858,71 @@
         <v>0</v>
       </c>
       <c r="M23" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N23" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O23" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R23" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S23" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U23" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V23" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W23" s="7">
+        <f t="shared" si="12"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z23">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA23">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC23">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD23">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE23">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N23" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O23" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q23" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R23" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S23" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40114305840163933</v>
-      </c>
-      <c r="U23" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V23" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ23">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W23" s="7">
-        <f t="shared" si="10"/>
-        <v>0.701171875</v>
-      </c>
-      <c r="Z23">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA23">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="24" spans="2:27">
+      <c r="AK23">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="24" spans="2:39">
       <c r="B24" s="3" t="s">
         <v>12</v>
       </c>
@@ -2456,51 +2951,71 @@
         <v>0</v>
       </c>
       <c r="M24" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N24" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O24" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R24" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S24" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U24" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V24" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W24" s="7">
+        <f t="shared" si="12"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z24">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA24">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC24">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD24">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE24">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N24" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O24" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q24" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R24" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S24" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40114305840163933</v>
-      </c>
-      <c r="U24" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V24" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ24">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W24" s="7">
-        <f t="shared" si="10"/>
-        <v>0.701171875</v>
-      </c>
-      <c r="Z24">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA24">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="25" spans="2:27">
+      <c r="AK24">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="25" spans="2:39">
       <c r="B25" s="3" t="s">
         <v>12</v>
       </c>
@@ -2529,51 +3044,71 @@
         <v>0</v>
       </c>
       <c r="M25" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N25" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O25" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R25" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S25" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U25" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V25" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W25" s="7">
+        <f t="shared" si="12"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z25">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA25">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC25">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD25">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE25">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N25" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O25" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q25" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R25" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S25" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40114305840163933</v>
-      </c>
-      <c r="U25" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V25" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ25">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W25" s="7">
-        <f t="shared" si="10"/>
-        <v>0.701171875</v>
-      </c>
-      <c r="Z25">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA25">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="26" spans="2:27">
+      <c r="AK25">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="26" spans="2:39">
       <c r="B26" s="3" t="s">
         <v>12</v>
       </c>
@@ -2602,51 +3137,71 @@
         <v>0</v>
       </c>
       <c r="M26" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N26" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O26" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q26" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R26" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S26" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40002241290983609</v>
+      </c>
+      <c r="U26" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V26" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W26" s="7">
+        <f t="shared" si="12"/>
+        <v>0.69921875</v>
+      </c>
+      <c r="Z26">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA26">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC26">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD26">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N26" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O26" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q26" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R26" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S26" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40002241290983609</v>
-      </c>
-      <c r="U26" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V26" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ26">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W26" s="7">
-        <f t="shared" si="10"/>
-        <v>0.69921875</v>
-      </c>
-      <c r="Z26">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA26">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="27" spans="2:27">
+      <c r="AK26">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="27" spans="2:39">
       <c r="B27" s="3" t="s">
         <v>12</v>
       </c>
@@ -2675,51 +3230,71 @@
         <v>0</v>
       </c>
       <c r="M27" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N27" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O27" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R27" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S27" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U27" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V27" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W27" s="7">
+        <f t="shared" si="12"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z27">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA27">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC27">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD27">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE27">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N27" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O27" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q27" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R27" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S27" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40114305840163933</v>
-      </c>
-      <c r="U27" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V27" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ27">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W27" s="7">
-        <f t="shared" si="10"/>
-        <v>0.701171875</v>
-      </c>
-      <c r="Z27">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA27">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="28" spans="2:27">
+      <c r="AK27">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="28" spans="2:39">
       <c r="B28" s="3" t="s">
         <v>12</v>
       </c>
@@ -2748,51 +3323,71 @@
         <v>0</v>
       </c>
       <c r="M28" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N28" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O28" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R28" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S28" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U28" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V28" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W28" s="7">
+        <f t="shared" si="12"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z28">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA28">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC28">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD28">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE28">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N28" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O28" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q28" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R28" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S28" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40114305840163933</v>
-      </c>
-      <c r="U28" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V28" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ28">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W28" s="7">
-        <f t="shared" si="10"/>
-        <v>0.701171875</v>
-      </c>
-      <c r="Z28">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA28">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="29" spans="2:27">
+      <c r="AK28">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="29" spans="2:39">
       <c r="B29" s="3" t="s">
         <v>12</v>
       </c>
@@ -2821,51 +3416,71 @@
         <v>0</v>
       </c>
       <c r="M29" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O29" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R29" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S29" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40114305840163933</v>
+      </c>
+      <c r="U29" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V29" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W29" s="7">
+        <f t="shared" si="12"/>
+        <v>0.701171875</v>
+      </c>
+      <c r="Z29">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA29">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC29">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD29">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE29">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N29" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O29" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q29" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R29" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S29" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40114305840163933</v>
-      </c>
-      <c r="U29" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V29" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ29">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W29" s="7">
-        <f t="shared" si="10"/>
-        <v>0.701171875</v>
-      </c>
-      <c r="Z29">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA29">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="30" spans="2:27">
+      <c r="AK29">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="30" spans="2:39">
       <c r="B30" s="3" t="s">
         <v>12</v>
       </c>
@@ -2894,51 +3509,71 @@
         <v>0</v>
       </c>
       <c r="M30" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N30" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O30" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q30" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.8027663934426229E-5</v>
+      </c>
+      <c r="R30" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4276543288934427</v>
+      </c>
+      <c r="S30" s="7">
+        <f t="shared" si="9"/>
+        <v>0.40002241290983609</v>
+      </c>
+      <c r="U30" s="7">
+        <f t="shared" si="10"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V30" s="7">
+        <f t="shared" si="11"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="W30" s="7">
+        <f t="shared" si="12"/>
+        <v>0.69921875</v>
+      </c>
+      <c r="Z30">
+        <f t="shared" si="15"/>
+        <v>0.24494250000000001</v>
+      </c>
+      <c r="AA30">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="AC30">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD30">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE30">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N30" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O30" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q30" s="7">
-        <f t="shared" si="5"/>
-        <v>-4.8027663934426229E-5</v>
-      </c>
-      <c r="R30" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4276543288934427</v>
-      </c>
-      <c r="S30" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40002241290983609</v>
-      </c>
-      <c r="U30" s="7">
-        <f t="shared" si="8"/>
-        <v>1.953125E-3</v>
-      </c>
-      <c r="V30" s="7">
-        <f t="shared" si="9"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ30">
+        <f t="shared" si="18"/>
         <v>2.490234375</v>
       </c>
-      <c r="W30" s="7">
-        <f t="shared" si="10"/>
-        <v>0.69921875</v>
-      </c>
-      <c r="Z30">
-        <f t="shared" si="12"/>
-        <v>0.24494250000000001</v>
-      </c>
-      <c r="AA30">
-        <f t="shared" si="11"/>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="31" spans="2:27">
+      <c r="AK30">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="31" spans="2:39">
       <c r="B31" s="3" t="s">
         <v>12</v>
       </c>
@@ -2979,19 +3614,19 @@
         <v>0</v>
       </c>
       <c r="Q31" s="7">
-        <f t="shared" ref="Q31:S31" si="13">($C31*E31+($C31*($C31-1))*H31/2-511)/512/854</f>
+        <f t="shared" ref="Q31:S31" si="20">($C31*E31+($C31*($C31-1))*H31/2-511)/512/854</f>
         <v>-4.8027663934426229E-5</v>
       </c>
       <c r="R31" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>1.4276543288934427</v>
       </c>
       <c r="S31" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>0.40114305840163933</v>
       </c>
       <c r="U31" s="7">
-        <f t="shared" ref="U31" si="14">(E31+$C31*H31)/512</f>
+        <f t="shared" ref="U31" si="21">(E31+$C31*H31)/512</f>
         <v>1.953125E-3</v>
       </c>
       <c r="V31" s="7">
@@ -3003,15 +3638,35 @@
         <v>0.701171875</v>
       </c>
       <c r="Z31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.24494250000000001</v>
       </c>
       <c r="AA31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>25000</v>
       </c>
-    </row>
-    <row r="32" spans="2:27">
+      <c r="AC31">
+        <f t="shared" si="16"/>
+        <v>490</v>
+      </c>
+      <c r="AD31">
+        <f t="shared" si="14"/>
+        <v>1220.21484375</v>
+      </c>
+      <c r="AE31">
+        <f t="shared" si="2"/>
+        <v>1220</v>
+      </c>
+      <c r="AJ31">
+        <f t="shared" si="18"/>
+        <v>2.490234375</v>
+      </c>
+      <c r="AK31">
+        <f t="shared" si="19"/>
+        <v>1220.21484375</v>
+      </c>
+    </row>
+    <row r="32" spans="2:39">
       <c r="B32" s="3" t="s">
         <v>12</v>
       </c>
@@ -3025,7 +3680,7 @@
         <v>127</v>
       </c>
       <c r="F32">
-        <v>1231</v>
+        <v>1236</v>
       </c>
       <c r="G32">
         <v>386</v>
@@ -3040,51 +3695,78 @@
         <v>-87</v>
       </c>
       <c r="M32" s="1">
-        <f t="shared" ref="M32" si="15">H32/512</f>
+        <f t="shared" ref="M32" si="22">H32/512</f>
         <v>0</v>
       </c>
       <c r="N32" s="1">
-        <f t="shared" ref="N32" si="16">I32/512</f>
+        <f t="shared" ref="N32" si="23">I32/512</f>
         <v>-0.603515625</v>
       </c>
       <c r="O32" s="1">
-        <f t="shared" ref="O32" si="17">J32/512</f>
+        <f t="shared" ref="O32" si="24">J32/512</f>
         <v>-0.169921875</v>
       </c>
       <c r="Q32" s="7">
-        <f t="shared" ref="Q32" si="18">($C32*E32+($C32*($C32-1))*H32/2-511)/512/854</f>
+        <f t="shared" ref="Q32" si="25">($C32*E32+($C32*($C32-1))*H32/2-511)/512/854</f>
         <v>-6.8610948477751756E-6</v>
       </c>
       <c r="R32" s="7">
-        <f t="shared" ref="R32" si="19">($C32*F32+($C32*($C32-1))*I32/2-511)/512/854</f>
-        <v>5.852513905152225E-3</v>
+        <f t="shared" ref="R32" si="26">($C32*F32+($C32*($C32-1))*I32/2-511)/512/854</f>
+        <v>5.8982545374707263E-3</v>
       </c>
       <c r="S32" s="7">
-        <f t="shared" ref="S32" si="20">($C32*G32+($C32*($C32-1))*J32/2-511)/512/854</f>
+        <f t="shared" ref="S32" si="27">($C32*G32+($C32*($C32-1))*J32/2-511)/512/854</f>
         <v>1.1686731557377049E-3</v>
       </c>
       <c r="U32" s="7">
-        <f t="shared" ref="U32" si="21">(E32+$C32*H32)/512</f>
+        <f t="shared" ref="U32" si="28">(E32+$C32*H32)/512</f>
         <v>0.248046875</v>
       </c>
       <c r="V32" s="7">
-        <f t="shared" ref="V32" si="22">(F32+$C32*I32)/512</f>
-        <v>-9.765625E-3</v>
+        <f t="shared" ref="V32" si="29">(F32+$C32*I32)/512</f>
+        <v>0</v>
       </c>
       <c r="W32" s="7">
-        <f t="shared" ref="W32" si="23">(G32+$C32*J32)/512</f>
+        <f t="shared" ref="W32" si="30">(G32+$C32*J32)/512</f>
         <v>7.421875E-2</v>
       </c>
       <c r="Z32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>1.9425E-3</v>
       </c>
       <c r="AA32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>24300</v>
       </c>
-    </row>
-    <row r="34" spans="2:26">
+      <c r="AC32">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="AD32">
+        <f t="shared" si="14"/>
+        <v>4.828125</v>
+      </c>
+      <c r="AE32">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AF32" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ32">
+        <f t="shared" si="18"/>
+        <v>2.4140625</v>
+      </c>
+      <c r="AK32">
+        <f>AJ32*4</f>
+        <v>9.65625</v>
+      </c>
+      <c r="AM32">
+        <f>(1236*4-309*4*4/2)/512</f>
+        <v>4.828125</v>
+      </c>
+    </row>
+    <row r="34" spans="2:33">
       <c r="C34">
         <f>SUM(C3:C33)</f>
         <v>13728</v>
@@ -3104,7 +3786,7 @@
       </c>
       <c r="R34" s="8">
         <f>SUM(R3:R31)</f>
-        <v>39.979002762734183</v>
+        <v>39.97739269247657</v>
       </c>
       <c r="S34" s="8">
         <f>SUM(S3:S31)</f>
@@ -3114,8 +3796,20 @@
         <f>SUM(Z3:Z33)</f>
         <v>6.8622749999999968</v>
       </c>
-    </row>
-    <row r="35" spans="2:26">
+      <c r="AD34">
+        <f>SUM(AD3:AD33)</f>
+        <v>34175.671875</v>
+      </c>
+      <c r="AE34">
+        <f>SUM(AE3:AE32)</f>
+        <v>34168</v>
+      </c>
+      <c r="AG34">
+        <f>34168/854</f>
+        <v>40.00936768149883</v>
+      </c>
+    </row>
+    <row r="35" spans="2:33">
       <c r="E35" t="s">
         <v>68</v>
       </c>
@@ -3125,8 +3819,16 @@
       <c r="G35" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="36" spans="2:26">
+      <c r="AD35">
+        <f>AD34/854</f>
+        <v>40.018351141686182</v>
+      </c>
+      <c r="AE35">
+        <f>AE34/854</f>
+        <v>40.00936768149883</v>
+      </c>
+    </row>
+    <row r="36" spans="2:33">
       <c r="F36">
         <v>50000000</v>
       </c>
@@ -3140,13 +3842,18 @@
         <v>38</v>
       </c>
       <c r="R36" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="S36" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="2:26">
+    <row r="37" spans="2:33">
+      <c r="AE37" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="2:33">
       <c r="B38" t="s">
         <v>41</v>
       </c>
@@ -3154,7 +3861,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="2:26">
+    <row r="39" spans="2:33">
       <c r="B39" t="s">
         <v>42</v>
       </c>
@@ -3162,19 +3869,37 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="2:26">
+    <row r="41" spans="2:33">
       <c r="F41" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="42" spans="2:26">
+      <c r="M41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="2:33">
       <c r="F42" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="43" spans="2:26">
+      <c r="M42" t="s">
+        <v>79</v>
+      </c>
+      <c r="O42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="2:33">
       <c r="F43" t="s">
         <v>67</v>
+      </c>
+      <c r="M43" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="2:33">
+      <c r="M45">
+        <f>490*1275/854/512</f>
+        <v>1.4288230020491803</v>
       </c>
     </row>
     <row r="49" spans="2:16">
@@ -5051,7 +5776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>

</xml_diff>